<commit_message>
changed id to xpath
</commit_message>
<xml_diff>
--- a/src/main/java/com/luma/testutil/LumaData.xlsx
+++ b/src/main/java/com/luma/testutil/LumaData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\eclipse-workspace\LUMA\src\main\java\com\luma\testutil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D226CF7A-B285-4E2B-9988-604934103759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A120DE-D604-416B-AAC6-80EB11655605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B5DACD30-F5D5-4982-BF6B-9441334A7FCC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B5DACD30-F5D5-4982-BF6B-9441334A7FCC}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -21,14 +21,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -60,16 +52,16 @@
     <t>C-Password</t>
   </si>
   <si>
-    <t>Charlie</t>
-  </si>
-  <si>
-    <t>Hebdo</t>
-  </si>
-  <si>
-    <t>charlie@gmail.com</t>
-  </si>
-  <si>
-    <t>Charlie#02</t>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>peterwh@gmail.com</t>
+  </si>
+  <si>
+    <t>Peter@26</t>
   </si>
 </sst>
 </file>
@@ -440,7 +432,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -450,15 +442,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E22A57CE-6810-498C-AEE7-4B6C6FB789B0}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -466,7 +458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -488,20 +480,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184F7CB0-B5B4-4184-BEC4-868252004E38}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -518,7 +510,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -528,16 +520,18 @@
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{9720DE2E-158D-4B93-8B44-91246DE26F7A}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{9301100D-21FC-44B7-88E0-21C9B4BA2D4A}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{95A72FF5-E374-4F70-A49D-DD46FD57A606}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>